<commit_message>
Roles adicionales agregados y diferenciados, dado que no son usuarios normales del sistema.
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Mapeo usuarios - roles.xlsx
+++ b/Docs/04-Requerimientos/Mapeo usuarios - roles.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Moderador de foro</t>
   </si>
@@ -67,13 +67,25 @@
   </si>
   <si>
     <t>Gestor evento citación</t>
+  </si>
+  <si>
+    <t>ADMINISTRADOR</t>
+  </si>
+  <si>
+    <t>DISEÑADOR WEB</t>
+  </si>
+  <si>
+    <t>ADL</t>
+  </si>
+  <si>
+    <t>Mensajero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,15 +101,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,12 +111,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -299,6 +316,109 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -307,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,31 +455,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,110 +798,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="87.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="87.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="30" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="H1" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="H2" s="32"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="18"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="28"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="33"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="B5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="33"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="25"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="1"/>
@@ -772,25 +930,31 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="33"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="25"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="33"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="25"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
@@ -799,56 +963,97 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="33"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="25"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="33"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="25"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="33"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="25"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J13" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lau - nada importante
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Mapeo usuarios - roles.xlsx
+++ b/Docs/04-Requerimientos/Mapeo usuarios - roles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de cambios" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Moderador de foro</t>
   </si>
@@ -141,6 +141,10 @@
   </si>
   <si>
     <t>Matriz de mapeo de roles con usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          Tipo de Usuario
+Roles</t>
   </si>
 </sst>
 </file>
@@ -389,17 +393,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="double">
         <color indexed="64"/>
       </bottom>
@@ -576,6 +569,19 @@
         <color indexed="64"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="medium">
+        <color indexed="64"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -608,56 +614,55 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -688,6 +693,9 @@
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,7 +1000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1005,92 +1013,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="34" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
+      <c r="A2" s="35"/>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="42"/>
+      <c r="B6" s="41"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="42" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="43" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="44">
         <v>40678</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="A10" s="45"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="51"/>
+      <c r="A13" s="47"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1102,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,119 +1120,121 @@
     <col min="2" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="87.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10"/>
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="18"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="27"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="28"/>
+      <c r="G3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="26"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="27"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="25"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="25"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="1"/>
@@ -1232,29 +1242,29 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="25"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="25"/>
+      <c r="G7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="32"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
@@ -1265,58 +1275,58 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="25"/>
+      <c r="G8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="32"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="24"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="25"/>
+      <c r="F9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="32"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="33"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="25"/>
+      <c r="B10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
@@ -1326,15 +1336,15 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="24"/>
+      <c r="F11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="32"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
@@ -1342,20 +1352,20 @@
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="17" t="s">
+      <c r="D12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="19"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J13" s="20"/>
+      <c r="J13" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregado de nuevos roles de mensajero
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Mapeo usuarios - roles.xlsx
+++ b/Docs/04-Requerimientos/Mapeo usuarios - roles.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>Moderador de foro</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>ADL</t>
-  </si>
-  <si>
-    <t>Mensajero</t>
   </si>
   <si>
     <t>Project Name:</t>
@@ -145,6 +142,15 @@
   <si>
     <t xml:space="preserve">                          Tipo de Usuario
 Roles</t>
+  </si>
+  <si>
+    <t>Mensajero alumno</t>
+  </si>
+  <si>
+    <t>Mensajero institución</t>
+  </si>
+  <si>
+    <t>Mensajero tutor</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1020,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1022,18 +1028,18 @@
     </row>
     <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1045,35 +1051,35 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="C8" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="D8" s="43" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="44">
         <v>40678</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1108,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,7 +1128,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>9</v>
@@ -1304,39 +1310,33 @@
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>15</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>15</v>
-      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="32"/>
       <c r="I10" s="22"/>
       <c r="J10" s="24"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="12" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="15" t="s">
@@ -1344,28 +1344,61 @@
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="32"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J13" s="19"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Detallle de User Stories y Actualizacion Matriz de Trazabilidad
</commit_message>
<xml_diff>
--- a/Docs/04-Requerimientos/Mapeo usuarios - roles.xlsx
+++ b/Docs/04-Requerimientos/Mapeo usuarios - roles.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="153">
   <si>
     <t>Moderador de foro</t>
   </si>
@@ -1372,6 +1372,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1387,24 +1405,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1820,8 +1820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,7 +1831,7 @@
     <col min="14" max="14" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:19" ht="109.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:19" ht="138" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="59" t="s">
         <v>33</v>
       </c>
@@ -2093,12 +2093,8 @@
       <c r="D12" s="71" t="s">
         <v>111</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="63"/>
       <c r="H12" s="62"/>
       <c r="I12" s="5" t="s">
@@ -2107,9 +2103,7 @@
       <c r="J12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="K12" s="37"/>
       <c r="L12" s="57"/>
       <c r="M12" s="8"/>
       <c r="N12" s="10"/>
@@ -2575,7 +2569,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="101" t="s">
+      <c r="C2" s="95" t="s">
         <v>102</v>
       </c>
       <c r="D2" s="39"/>
@@ -2591,7 +2585,7 @@
       <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C3" s="101"/>
+      <c r="C3" s="95"/>
       <c r="D3" s="39" t="s">
         <v>86</v>
       </c>
@@ -2618,18 +2612,18 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="92" t="s">
+      <c r="A5" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="97" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="67" t="s">
@@ -2653,8 +2647,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
-      <c r="B6" s="103"/>
+      <c r="A6" s="99"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="67" t="s">
         <v>89</v>
       </c>
@@ -2674,8 +2668,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="93"/>
-      <c r="B7" s="103"/>
+      <c r="A7" s="99"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="67" t="s">
         <v>88</v>
       </c>
@@ -2697,8 +2691,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="93"/>
-      <c r="B8" s="103"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="67" t="s">
         <v>87</v>
       </c>
@@ -2722,8 +2716,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="93"/>
-      <c r="B9" s="95" t="s">
+      <c r="A9" s="99"/>
+      <c r="B9" s="101" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="67" t="s">
@@ -2749,8 +2743,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="93"/>
-      <c r="B10" s="96"/>
+      <c r="A10" s="99"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="67" t="s">
         <v>40</v>
       </c>
@@ -2774,8 +2768,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="93"/>
-      <c r="B11" s="96"/>
+      <c r="A11" s="99"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="67" t="s">
         <v>41</v>
       </c>
@@ -2799,8 +2793,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="93"/>
-      <c r="B12" s="96"/>
+      <c r="A12" s="99"/>
+      <c r="B12" s="102"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -2811,8 +2805,8 @@
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="93"/>
-      <c r="B13" s="97"/>
+      <c r="A13" s="99"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="67"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -2824,8 +2818,8 @@
       <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="93"/>
-      <c r="B14" s="95" t="s">
+      <c r="A14" s="99"/>
+      <c r="B14" s="101" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="67" t="s">
@@ -2849,8 +2843,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="93"/>
-      <c r="B15" s="96"/>
+      <c r="A15" s="99"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="67" t="s">
         <v>42</v>
       </c>
@@ -2872,8 +2866,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="93"/>
-      <c r="B16" s="97"/>
+      <c r="A16" s="99"/>
+      <c r="B16" s="103"/>
       <c r="C16" s="67" t="s">
         <v>131</v>
       </c>
@@ -2893,8 +2887,8 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="93"/>
-      <c r="B17" s="95" t="s">
+      <c r="A17" s="99"/>
+      <c r="B17" s="101" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="67" t="s">
@@ -2914,8 +2908,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="93"/>
-      <c r="B18" s="96"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="102"/>
       <c r="C18" s="67" t="s">
         <v>48</v>
       </c>
@@ -2933,8 +2927,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="93"/>
-      <c r="B19" s="96"/>
+      <c r="A19" s="99"/>
+      <c r="B19" s="102"/>
       <c r="C19" s="67" t="s">
         <v>49</v>
       </c>
@@ -2952,8 +2946,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="93"/>
-      <c r="B20" s="96"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="67" t="s">
         <v>50</v>
       </c>
@@ -2971,8 +2965,8 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="93"/>
-      <c r="B21" s="96"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="102"/>
       <c r="C21" s="67" t="s">
         <v>51</v>
       </c>
@@ -2990,8 +2984,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="93"/>
-      <c r="B22" s="96"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="67" t="s">
         <v>52</v>
       </c>
@@ -3009,7 +3003,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="94"/>
+      <c r="A23" s="100"/>
       <c r="B23" s="73"/>
       <c r="C23" s="88"/>
       <c r="D23" s="8"/>
@@ -3021,7 +3015,7 @@
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="95" t="s">
+      <c r="A24" s="101" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="70" t="s">
@@ -3040,7 +3034,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="96"/>
+      <c r="A25" s="102"/>
       <c r="B25" s="70" t="s">
         <v>43</v>
       </c>
@@ -3057,7 +3051,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="96"/>
+      <c r="A26" s="102"/>
       <c r="B26" s="70" t="s">
         <v>44</v>
       </c>
@@ -3074,7 +3068,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="96"/>
+      <c r="A27" s="102"/>
       <c r="B27" s="70" t="s">
         <v>45</v>
       </c>
@@ -3091,7 +3085,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="96"/>
+      <c r="A28" s="102"/>
       <c r="B28" s="70"/>
       <c r="C28" s="88"/>
       <c r="D28" s="8"/>
@@ -3104,7 +3098,7 @@
       <c r="L28" s="8"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="97"/>
+      <c r="A29" s="103"/>
       <c r="B29" s="70" t="s">
         <v>140</v>
       </c>
@@ -3137,7 +3131,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="92" t="s">
+      <c r="A31" s="98" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="69" t="s">
@@ -3157,7 +3151,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="93"/>
+      <c r="A32" s="99"/>
       <c r="B32" s="70" t="s">
         <v>137</v>
       </c>
@@ -3177,7 +3171,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
+      <c r="A33" s="100"/>
       <c r="B33" s="70" t="s">
         <v>60</v>
       </c>
@@ -3215,7 +3209,7 @@
       <c r="L34" s="8"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="92" t="s">
+      <c r="A35" s="98" t="s">
         <v>55</v>
       </c>
       <c r="B35" s="70" t="s">
@@ -3238,7 +3232,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="93"/>
+      <c r="A36" s="99"/>
       <c r="B36" s="70" t="s">
         <v>62</v>
       </c>
@@ -3259,7 +3253,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="93"/>
+      <c r="A37" s="99"/>
       <c r="B37" s="70" t="s">
         <v>63</v>
       </c>
@@ -3280,7 +3274,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="93"/>
+      <c r="A38" s="99"/>
       <c r="B38" s="70" t="s">
         <v>98</v>
       </c>
@@ -3305,7 +3299,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="93"/>
+      <c r="A39" s="99"/>
       <c r="B39" s="70" t="s">
         <v>64</v>
       </c>
@@ -3330,7 +3324,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="94"/>
+      <c r="A40" s="100"/>
       <c r="B40" s="70" t="s">
         <v>65</v>
       </c>
@@ -3411,10 +3405,10 @@
       <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="92" t="s">
+      <c r="A45" s="98" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="92" t="s">
         <v>96</v>
       </c>
       <c r="C45" s="67" t="s">
@@ -3440,8 +3434,8 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="93"/>
-      <c r="B46" s="99"/>
+      <c r="A46" s="99"/>
+      <c r="B46" s="93"/>
       <c r="C46" s="67" t="s">
         <v>147</v>
       </c>
@@ -3461,8 +3455,8 @@
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="93"/>
-      <c r="B47" s="99"/>
+      <c r="A47" s="99"/>
+      <c r="B47" s="93"/>
       <c r="C47" s="67"/>
       <c r="D47" s="8" t="s">
         <v>74</v>
@@ -3482,8 +3476,8 @@
       <c r="L47" s="89"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="93"/>
-      <c r="B48" s="100"/>
+      <c r="A48" s="99"/>
+      <c r="B48" s="94"/>
       <c r="C48" s="67"/>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
@@ -3499,7 +3493,7 @@
       <c r="L48" s="89"/>
     </row>
     <row r="49" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="93"/>
+      <c r="A49" s="99"/>
       <c r="B49" s="70" t="s">
         <v>93</v>
       </c>
@@ -3518,7 +3512,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="93"/>
+      <c r="A50" s="99"/>
       <c r="B50" s="70" t="s">
         <v>94</v>
       </c>
@@ -3539,7 +3533,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="94"/>
+      <c r="A51" s="100"/>
       <c r="B51" s="70" t="s">
         <v>95</v>
       </c>
@@ -3558,7 +3552,7 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" s="92" t="s">
+      <c r="A52" s="98" t="s">
         <v>57</v>
       </c>
       <c r="B52" s="70" t="s">
@@ -3588,7 +3582,7 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="94"/>
+      <c r="A53" s="100"/>
       <c r="B53" s="70" t="s">
         <v>67</v>
       </c>
@@ -3621,7 +3615,7 @@
       <c r="L54" s="8"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="92" t="s">
+      <c r="A55" s="98" t="s">
         <v>68</v>
       </c>
       <c r="B55" s="70" t="s">
@@ -3653,7 +3647,7 @@
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="93"/>
+      <c r="A56" s="99"/>
       <c r="B56" s="70" t="s">
         <v>70</v>
       </c>
@@ -3679,7 +3673,7 @@
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="94"/>
+      <c r="A57" s="100"/>
       <c r="B57" s="70" t="s">
         <v>71</v>
       </c>
@@ -3736,7 +3730,7 @@
       <c r="L59" s="8"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="92" t="s">
+      <c r="A60" s="98" t="s">
         <v>72</v>
       </c>
       <c r="B60" s="70" t="s">
@@ -3763,7 +3757,7 @@
       </c>
     </row>
     <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="94"/>
+      <c r="A61" s="100"/>
       <c r="B61" s="70" t="s">
         <v>100</v>
       </c>
@@ -3987,6 +3981,13 @@
   </sheetData>
   <autoFilter ref="L1:L78"/>
   <mergeCells count="15">
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A45:A51"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="A4:C4"/>
@@ -3995,13 +3996,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B17:B22"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A45:A51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>